<commit_message>
trying to optimalize classifier
</commit_message>
<xml_diff>
--- a/Semester II/Masterproef/logboek/logboek.xlsx
+++ b/Semester II/Masterproef/logboek/logboek.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2637A38B-3417-4E27-A15E-42C13AB003B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FF1D32-3158-413F-B7F5-758796B438A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="63">
   <si>
     <t>Week 1</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Simple Buffer classificatie</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>Week 15</t>
   </si>
 </sst>
 </file>
@@ -649,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,6 +675,9 @@
     <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="56" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="56" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -743,10 +755,12 @@
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="7"/>
+      <c r="P4" s="9"/>
       <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -786,10 +800,18 @@
       <c r="L5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="M5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="4">
+        <v>43591</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -827,10 +849,18 @@
       <c r="L6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="M6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="4">
+        <v>43592</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -870,10 +900,18 @@
       <c r="L7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="M7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="4">
+        <v>43593</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -913,10 +951,18 @@
       <c r="L8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="M8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="4">
+        <v>43594</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -954,10 +1000,18 @@
       <c r="L9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="M9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="4">
+        <v>43595</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -995,10 +1049,16 @@
         <v>2</v>
       </c>
       <c r="L10" s="2"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="M10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="4">
+        <v>43596</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1036,10 +1096,16 @@
         <v>2</v>
       </c>
       <c r="L11" s="2"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="M11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="4">
+        <v>43597</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2"/>
       <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1070,10 +1136,15 @@
         <v>4</v>
       </c>
       <c r="L12" s="2"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="5">
+        <f>SUM(O5:O11)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="2"/>
       <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1095,10 +1166,12 @@
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="9"/>
       <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1138,10 +1211,16 @@
       <c r="L14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="M14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="4">
+        <v>43598</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2"/>
       <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1181,10 +1260,16 @@
       <c r="L15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="M15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="4">
+        <v>43599</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2"/>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1224,10 +1309,16 @@
       <c r="L16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="M16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="4">
+        <v>43600</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1267,10 +1358,16 @@
       <c r="L17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="M17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N17" s="4">
+        <v>43601</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1310,10 +1407,16 @@
       <c r="L18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="M18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="4">
+        <v>43602</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2"/>
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1353,6 +1456,16 @@
       <c r="L19" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="M19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="4">
+        <v>43603</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1390,6 +1503,15 @@
       </c>
       <c r="L20" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="4">
+        <v>43604</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1420,6 +1542,15 @@
         <v>7</v>
       </c>
       <c r="L21" s="2"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="5">
+        <f>SUM(O14:O20)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
@@ -1440,6 +1571,12 @@
       </c>
       <c r="K22" s="7"/>
       <c r="L22" s="9"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="9"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1478,6 +1615,17 @@
       <c r="L23" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="M23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" s="4">
+        <f>N20+1</f>
+        <v>43605</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1516,6 +1664,17 @@
       <c r="L24" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="M24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N24" s="4">
+        <f>N23+1</f>
+        <v>43606</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1554,6 +1713,17 @@
       <c r="L25" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="M25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" ref="N25:N29" si="0">N24+1</f>
+        <v>43607</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1592,6 +1762,17 @@
       <c r="L26" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="M26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N26" s="4">
+        <f t="shared" si="0"/>
+        <v>43608</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1630,6 +1811,17 @@
       <c r="L27" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="M27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N27" s="4">
+        <f t="shared" si="0"/>
+        <v>43609</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1668,6 +1860,17 @@
       <c r="L28" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="M28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="0"/>
+        <v>43610</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1704,6 +1907,17 @@
         <v>0</v>
       </c>
       <c r="L29" s="2"/>
+      <c r="M29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N29" s="4">
+        <f t="shared" si="0"/>
+        <v>43611</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
@@ -1733,6 +1947,15 @@
         <v>17</v>
       </c>
       <c r="L30" s="2"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O30" s="5">
+        <f>SUM(O23:O29)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
@@ -1753,6 +1976,12 @@
       </c>
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O31" s="7"/>
+      <c r="P31" s="9"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1789,8 +2018,19 @@
       <c r="L32" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" s="4">
+        <f>N29+1</f>
+        <v>43612</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1825,8 +2065,19 @@
       <c r="L33" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N33" s="4">
+        <f>N32+1</f>
+        <v>43613</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1861,8 +2112,19 @@
       <c r="L34" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" s="4">
+        <f t="shared" ref="N34:N38" si="1">N33+1</f>
+        <v>43614</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -1895,8 +2157,19 @@
         <v>0</v>
       </c>
       <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N35" s="4">
+        <f t="shared" si="1"/>
+        <v>43615</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
@@ -1931,8 +2204,19 @@
         <v>0</v>
       </c>
       <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="4">
+        <f t="shared" si="1"/>
+        <v>43616</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -1967,8 +2251,19 @@
         <v>0</v>
       </c>
       <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N37" s="4">
+        <f t="shared" si="1"/>
+        <v>43617</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
@@ -2003,8 +2298,19 @@
         <v>0</v>
       </c>
       <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N38" s="4">
+        <f t="shared" si="1"/>
+        <v>43618</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="14" t="s">
         <v>23</v>
@@ -2032,6 +2338,15 @@
         <v>14</v>
       </c>
       <c r="L39" s="16"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O39" s="15">
+        <f>SUM(O32:O38)</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>